<commit_message>
cleaned up names of fit files
</commit_message>
<xml_diff>
--- a/fits/ver4/model_parameters.xlsx
+++ b/fits/ver4/model_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="17115" windowHeight="6915"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="17115" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
-  <si>
-    <t>name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="102">
   <si>
     <t>fit1</t>
   </si>
@@ -186,9 +183,6 @@
     <t>fit7</t>
   </si>
   <si>
-    <t>fit8</t>
-  </si>
-  <si>
     <t>19458</t>
   </si>
   <si>
@@ -325,6 +319,9 @@
   </si>
   <si>
     <t>40.6</t>
+  </si>
+  <si>
+    <t>fit3</t>
   </si>
 </sst>
 </file>
@@ -334,23 +331,8 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -384,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,20 +377,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,134 +680,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5">
+        <v>11996</v>
+      </c>
+      <c r="C2" s="5">
+        <v>9664</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="5">
+        <v>8827</v>
+      </c>
+      <c r="F2" s="5">
+        <v>8525</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="4">
+        <v>40.6</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="6">
-        <v>11996</v>
-      </c>
-      <c r="C2" s="6">
-        <v>9664</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="5">
-        <v>8827</v>
-      </c>
-      <c r="G2" s="6">
-        <v>8525</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G3" s="8">
-        <v>40.6</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>20.399999999999999</v>
@@ -839,27 +803,25 @@
       <c r="C5" s="2">
         <v>24.2</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3" t="s">
-        <v>58</v>
+      <c r="D5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="2">
+        <v>21.5</v>
       </c>
       <c r="F5" s="2">
         <v>21.5</v>
       </c>
-      <c r="G5" s="2">
-        <v>21.5</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
+      <c r="G5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>98.5</v>
@@ -867,55 +829,51 @@
       <c r="C6" s="2">
         <v>118.8</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="2">
+        <v>102.9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="2">
-        <v>102.9</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="4" t="s">
+      <c r="C7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8:C8" si="0">DEGREES(ATAN(B5/B6))</f>
@@ -925,32 +883,30 @@
         <f t="shared" si="0"/>
         <v>11.51383118448701</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <f>DEGREES(ATAN(D5/D6))</f>
+        <v>13.423165532178205</v>
+      </c>
       <c r="E8" s="2">
         <f>DEGREES(ATAN(E5/E6))</f>
-        <v>13.423165532178205</v>
+        <v>11.680260148566321</v>
       </c>
       <c r="F8" s="2">
         <f>DEGREES(ATAN(F5/F6))</f>
-        <v>11.680260148566321</v>
+        <v>11.801637913264774</v>
       </c>
       <c r="G8" s="2">
-        <f>DEGREES(ATAN(G5/G6))</f>
-        <v>11.801637913264774</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2">
-        <f t="shared" ref="I8:J8" si="1">DEGREES(ATAN(I5/I6))</f>
+        <f t="shared" ref="G8:H8" si="1">DEGREES(ATAN(G5/G6))</f>
         <v>11.837741043343341</v>
       </c>
-      <c r="J8" s="2">
+      <c r="H8" s="2">
         <f t="shared" si="1"/>
         <v>11.82397427342039</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="4" t="s">
-        <v>8</v>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9:C9" si="2">DEGREES(ATAN(B5/(B7-B6)))</f>
@@ -960,340 +916,316 @@
         <f t="shared" si="2"/>
         <v>42.727550267217062</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <f>DEGREES(ATAN(D5/(D7-D6)))</f>
+        <v>22.867863527024735</v>
+      </c>
       <c r="E9" s="2">
         <f>DEGREES(ATAN(E5/(E7-E6)))</f>
-        <v>22.867863527024735</v>
+        <v>27.67207822275877</v>
       </c>
       <c r="F9" s="2">
         <f>DEGREES(ATAN(F5/(F7-F6)))</f>
-        <v>27.67207822275877</v>
+        <v>27.052893707269813</v>
       </c>
       <c r="G9" s="2">
-        <f>DEGREES(ATAN(G5/(G7-G6)))</f>
-        <v>27.052893707269813</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2">
-        <f t="shared" ref="I9:J9" si="3">DEGREES(ATAN(I5/(I7-I6)))</f>
+        <f t="shared" ref="G9:H9" si="3">DEGREES(ATAN(G5/(G7-G6)))</f>
         <v>26.51160363706509</v>
       </c>
-      <c r="J9" s="2">
+      <c r="H9" s="2">
         <f t="shared" si="3"/>
         <v>26.943057432991445</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
+    <row r="10" spans="1:8">
+      <c r="A10" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B10" s="3">
         <v>0.48899999999999999</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="4" t="s">
+      <c r="F11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="B12" s="3">
         <v>0.26600000000000001</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="E12" s="3" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>85</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="B13" s="3">
         <v>19.8</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="G13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="E14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="E15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="3">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="4" t="s">
+      <c r="H16" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3" t="s">
+      <c r="E19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="3">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="H19" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J18" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
done some more fits
</commit_message>
<xml_diff>
--- a/fits/ver4/model_parameters.xlsx
+++ b/fits/ver4/model_parameters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
   <si>
     <t>fit1</t>
   </si>
@@ -322,6 +322,18 @@
   </si>
   <si>
     <t>fit3</t>
+  </si>
+  <si>
+    <t>fit8</t>
+  </si>
+  <si>
+    <t>fit9</t>
+  </si>
+  <si>
+    <t>fit10</t>
+  </si>
+  <si>
+    <t>Sun et al</t>
   </si>
 </sst>
 </file>
@@ -680,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -691,7 +703,7 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" s="6"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -714,8 +726,20 @@
       <c r="H1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -740,8 +764,17 @@
       <c r="H2" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="1">
+        <v>1364</v>
+      </c>
+      <c r="J2" s="1">
+        <v>889</v>
+      </c>
+      <c r="K2" s="1">
+        <v>8131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="6" t="s">
         <v>95</v>
       </c>
@@ -766,8 +799,20 @@
       <c r="H3" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="1">
+        <v>38</v>
+      </c>
+      <c r="J3" s="1">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="K3" s="1">
+        <v>41.8</v>
+      </c>
+      <c r="L3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
         <v>96</v>
       </c>
@@ -792,8 +837,20 @@
       <c r="H4" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="1">
+        <v>28.6</v>
+      </c>
+      <c r="J4" s="1">
+        <v>31.4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="L4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -818,8 +875,20 @@
       <c r="H5" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="1">
+        <v>24.9</v>
+      </c>
+      <c r="J5" s="2">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K5" s="1">
+        <v>20.6</v>
+      </c>
+      <c r="L5" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -844,8 +913,20 @@
       <c r="H6" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="1">
+        <v>121.7</v>
+      </c>
+      <c r="J6" s="1">
+        <v>103.2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>101</v>
+      </c>
+      <c r="L6" s="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -870,8 +951,20 @@
       <c r="H7" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="1">
+        <v>141.69999999999999</v>
+      </c>
+      <c r="K7" s="1">
+        <v>145</v>
+      </c>
+      <c r="L7" s="1">
+        <v>141.69999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -896,15 +989,31 @@
         <v>11.801637913264774</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" ref="G8:H8" si="1">DEGREES(ATAN(G5/G6))</f>
+        <f t="shared" ref="G8:L8" si="1">DEGREES(ATAN(G5/G6))</f>
         <v>11.837741043343341</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="1"/>
         <v>11.82397427342039</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>11.563211819838829</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>10.753680246939542</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="1"/>
+        <v>11.527951891752842</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="1"/>
+        <v>10.451632943988697</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -929,15 +1038,31 @@
         <v>27.052893707269813</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" ref="G9:H9" si="3">DEGREES(ATAN(G5/(G7-G6)))</f>
+        <f t="shared" ref="G9:L9" si="3">DEGREES(ATAN(G5/(G7-G6)))</f>
         <v>26.51160363706509</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="3"/>
         <v>26.943057432991445</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="2">
+        <f t="shared" si="3"/>
+        <v>46.901236464614435</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="3"/>
+        <v>26.980230718222863</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>25.088139125926986</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="3"/>
+        <v>26.149010297836654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -962,8 +1087,18 @@
       <c r="H10" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="1">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
@@ -988,8 +1123,18 @@
       <c r="H11" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="1">
+        <v>-9.75</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-2.12</v>
+      </c>
+      <c r="K11" s="1">
+        <v>-2.48</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -1014,8 +1159,20 @@
       <c r="H12" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="1">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
@@ -1040,8 +1197,20 @@
       <c r="H13" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" s="1">
+        <v>19.7</v>
+      </c>
+      <c r="J13" s="1">
+        <v>19.2</v>
+      </c>
+      <c r="K13" s="1">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="L13" s="1">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
@@ -1066,8 +1235,17 @@
       <c r="H14" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="1">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
@@ -1092,8 +1270,17 @@
       <c r="H15" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -1118,8 +1305,17 @@
       <c r="H16" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="1">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
@@ -1144,8 +1340,17 @@
       <c r="H17" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="1">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1170,8 +1375,17 @@
       <c r="H18" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="1">
+        <v>6.58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
@@ -1196,8 +1410,17 @@
       <c r="H19" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="6" t="s">
         <v>16</v>
       </c>
@@ -1221,6 +1444,15 @@
       </c>
       <c r="H20" s="3" t="s">
         <v>79</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="1">
+        <v>9.7899999999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>